<commit_message>
Create a Roll-Up Summary Field
</commit_message>
<xml_diff>
--- a/1.approval-process/3.Build-a-Travel-Approval-App/3.Add-Business-Logic-to-a-Travel-Approval-App.xlsx
+++ b/1.approval-process/3.Build-a-Travel-Approval-App/3.Add-Business-Logic-to-a-Travel-Approval-App.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\salesforce-trailhead\1.approval-process\3.Build-a-Travel-Approval-App\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7787AD95-ECD2-4162-994C-D2D4D1AC9D16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43718918-D114-4E7A-BD8E-4DA2904602F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Create Validation Rules" sheetId="1" r:id="rId1"/>
+    <sheet name="Create a Roll-Up Summary Field" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,9 +26,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>https://trailhead.salesforce.com/content/learn/projects/add-business-logic-to-a-travel-approval-app/create-validation-rules-travel?trail_id=build-a-travel-approval-app</t>
+  </si>
+  <si>
+    <t>https://trailhead.salesforce.com/content/learn/projects/add-business-logic-to-a-travel-approval-app/create-a-rollup-summary-field-travel?trail_id=build-a-travel-approval-app</t>
   </si>
 </sst>
 </file>
@@ -441,6 +445,457 @@
         <a:xfrm>
           <a:off x="739589" y="59167059"/>
           <a:ext cx="11205882" cy="4848225"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>114299</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>180974</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>109566</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{64E15E34-BF12-CB58-98CC-119B186994C7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="723899" y="666750"/>
+          <a:ext cx="11039475" cy="10682316"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>86</xdr:row>
+      <xdr:rowOff>17383</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E907F280-CF7D-1EEE-BF9B-2556F739D3E8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="733425" y="11525250"/>
+          <a:ext cx="11268075" cy="4875133"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>87</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>285750</xdr:colOff>
+      <xdr:row>113</xdr:row>
+      <xdr:rowOff>187502</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{871C342B-4F48-5D86-8B19-29B665EC7135}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="755196" y="16668750"/>
+          <a:ext cx="11164661" cy="5045252"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>115</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>428625</xdr:colOff>
+      <xdr:row>142</xdr:row>
+      <xdr:rowOff>54438</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F0A0FF1E-44CD-2D01-90AC-8234F9F2B763}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="723900" y="21974175"/>
+          <a:ext cx="11287125" cy="5131263"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>143</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>400050</xdr:colOff>
+      <xdr:row>170</xdr:row>
+      <xdr:rowOff>70887</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D8CFEE42-8548-216A-88B4-BEFA6D7E1615}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="742950" y="27346275"/>
+          <a:ext cx="11239500" cy="5109612"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>152401</xdr:colOff>
+      <xdr:row>171</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>190501</xdr:colOff>
+      <xdr:row>194</xdr:row>
+      <xdr:rowOff>93154</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A2E76A67-48BD-03C6-7352-196C2D3312B2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="764722" y="32632650"/>
+          <a:ext cx="11059886" cy="4417504"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>195</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>353786</xdr:colOff>
+      <xdr:row>222</xdr:row>
+      <xdr:rowOff>59209</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Picture 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B5F45933-A3CD-F7BB-1ECF-04378847533B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="698046" y="37223700"/>
+          <a:ext cx="11289847" cy="5126509"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>223</xdr:row>
+      <xdr:rowOff>57151</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>369794</xdr:colOff>
+      <xdr:row>250</xdr:row>
+      <xdr:rowOff>51305</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="Picture 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8BC527EA-2257-C30B-19F5-05CD8352C780}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="719418" y="42538651"/>
+          <a:ext cx="11147611" cy="5137654"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>100853</xdr:colOff>
+      <xdr:row>251</xdr:row>
+      <xdr:rowOff>89648</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>313765</xdr:colOff>
+      <xdr:row>277</xdr:row>
+      <xdr:rowOff>55054</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="Picture 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1EF50E2F-B43A-E0A2-7C61-C2FFFB1B1569}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="705971" y="47905148"/>
+          <a:ext cx="11105029" cy="4918406"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>145676</xdr:colOff>
+      <xdr:row>278</xdr:row>
+      <xdr:rowOff>145677</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>336177</xdr:colOff>
+      <xdr:row>304</xdr:row>
+      <xdr:rowOff>182289</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="12" name="Picture 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6BFF56B7-B1B7-0601-9BCD-3971409E65C4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="750794" y="53104677"/>
+          <a:ext cx="11082618" cy="4989612"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -717,8 +1172,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A325" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H343" sqref="H343"/>
+    <sheetView topLeftCell="A325" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H346" sqref="H346"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -732,4 +1187,25 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68346350-4204-4C58-99AC-5AB213CA5A5F}">
+  <dimension ref="B3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A287" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B279" sqref="B279"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B3" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>